<commit_message>
bulk upload 11 12 25
</commit_message>
<xml_diff>
--- a/resources/excel/example.xlsx
+++ b/resources/excel/example.xlsx
@@ -786,9 +786,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="d\-m"/>
+    <numFmt numFmtId="166" formatCode="d, m"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -838,7 +839,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -880,6 +881,9 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1102,6 +1106,12 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="15" max="15" width="22.0"/>
+    <col customWidth="1" min="18" max="18" width="66.38"/>
+    <col customWidth="1" min="25" max="25" width="21.25"/>
+    <col customWidth="1" min="26" max="26" width="18.13"/>
+  </cols>
   <sheetData>
     <row r="1" ht="15.0" customHeight="1">
       <c r="A1" s="1" t="s">
@@ -4235,8 +4245,8 @@
       <c r="E37" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="F37" s="3">
-        <v>2.6</v>
+      <c r="F37" s="14">
+        <v>45810.0</v>
       </c>
       <c r="G37" s="3">
         <v>1.0</v>
@@ -5196,10 +5206,10 @@
       <c r="J48" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K48" s="14" t="s">
+      <c r="K48" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="L48" s="14" t="s">
+      <c r="L48" s="15" t="s">
         <v>180</v>
       </c>
       <c r="M48" s="2" t="s">
@@ -5211,10 +5221,10 @@
       <c r="O48" s="3">
         <v>8.0</v>
       </c>
-      <c r="P48" s="15">
+      <c r="P48" s="16">
         <v>49.0146395418681</v>
       </c>
-      <c r="Q48" s="15">
+      <c r="Q48" s="16">
         <v>21.2208887255057</v>
       </c>
       <c r="R48" s="6" t="s">
@@ -5282,10 +5292,10 @@
       <c r="J49" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K49" s="14" t="s">
+      <c r="K49" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="L49" s="14" t="s">
+      <c r="L49" s="15" t="s">
         <v>182</v>
       </c>
       <c r="M49" s="2" t="s">
@@ -5297,10 +5307,10 @@
       <c r="O49" s="3">
         <v>9.0</v>
       </c>
-      <c r="P49" s="15">
+      <c r="P49" s="16">
         <v>49.0146395418681</v>
       </c>
-      <c r="Q49" s="15">
+      <c r="Q49" s="16">
         <v>21.2208887255057</v>
       </c>
       <c r="R49" s="6" t="s">
@@ -5368,10 +5378,10 @@
       <c r="J50" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K50" s="14" t="s">
+      <c r="K50" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="L50" s="14" t="s">
+      <c r="L50" s="15" t="s">
         <v>183</v>
       </c>
       <c r="M50" s="2" t="s">
@@ -5383,10 +5393,10 @@
       <c r="O50" s="3">
         <v>8.0</v>
       </c>
-      <c r="P50" s="15">
+      <c r="P50" s="16">
         <v>49.0146395418681</v>
       </c>
-      <c r="Q50" s="15">
+      <c r="Q50" s="16">
         <v>21.2208887255057</v>
       </c>
       <c r="R50" s="6" t="s">
@@ -5454,10 +5464,10 @@
       <c r="J51" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="K51" s="14" t="s">
+      <c r="K51" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="L51" s="14" t="s">
+      <c r="L51" s="15" t="s">
         <v>185</v>
       </c>
       <c r="M51" s="2" t="s">
@@ -5469,10 +5479,10 @@
       <c r="O51" s="3">
         <v>10.0</v>
       </c>
-      <c r="P51" s="15">
+      <c r="P51" s="16">
         <v>49.0146395418681</v>
       </c>
-      <c r="Q51" s="15">
+      <c r="Q51" s="16">
         <v>21.2208887255057</v>
       </c>
       <c r="R51" s="6" t="s">
@@ -7847,8 +7857,8 @@
       <c r="E79" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="F79" s="3">
-        <v>2.6</v>
+      <c r="F79" s="14">
+        <v>45810.0</v>
       </c>
       <c r="G79" s="3">
         <v>1.0</v>
@@ -8711,8 +8721,8 @@
       <c r="E89" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F89" s="3">
-        <v>2.6</v>
+      <c r="F89" s="14">
+        <v>45810.0</v>
       </c>
       <c r="G89" s="3">
         <v>1.0</v>

</xml_diff>